<commit_message>
Delete sample added. ISO dates.
</commit_message>
<xml_diff>
--- a/Example/Example.xlsx
+++ b/Example/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanita\Desktop\sand-granulomety\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194A1F66-1D29-44AD-8879-B959CA03E641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48AB02F-4873-449E-987F-D99D4C17BB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1140" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -223,6 +223,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,8 +264,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -546,12 +549,12 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -632,37 +635,37 @@
       <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>36607</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>0.68965517241379315</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>6.8965517241379306</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>8.2758620689655178</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>15.862068965517242</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>25.517241379310345</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>13.793103448275861</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>12.413793103448276</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>8.9655172413793096</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>6.2068965517241379</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>1.3793103448275863</v>
       </c>
     </row>
@@ -688,37 +691,37 @@
       <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>36607</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>4.4334975369458132</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>10.344827586206897</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>14.77832512315271</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>22.167487684729064</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="2">
         <v>19.21182266009852</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>9.8522167487684733</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="2">
         <v>7.8817733990147785</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="2">
         <v>7.389162561576355</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <v>3.4482758620689653</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="2">
         <v>0.49261083743842365</v>
       </c>
     </row>
@@ -744,37 +747,37 @@
       <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>36607</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>0.19801980198019803</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>2.6402640264026402</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>10.561056105610561</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>16.5016501650165</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>20.462046204620464</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>19.141914191419144</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>16.5016501650165</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>11.221122112211221</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>2.6402640264026402</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <v>0.132013201320132</v>
       </c>
     </row>
@@ -800,37 +803,37 @@
       <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>36608</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>0.33783783783783783</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>3.7162162162162162</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>9.4594594594594597</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>15.202702702702704</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>18.918918918918919</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>16.216216216216218</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>13.851351351351351</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>13.513513513513514</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>7.4324324324324325</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="2">
         <v>1.3513513513513513</v>
       </c>
     </row>
@@ -856,37 +859,37 @@
       <c r="G6" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>40338</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>8.1234768480909839E-2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>1.2185215272136476</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>8.9358245329000816</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>16.246953696181968</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>17.871649065800163</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>18.277822908204712</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <v>17.059301380991066</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>14.62225832656377</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <v>4.8740861088545904</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <v>0.81234768480909836</v>
       </c>
     </row>
@@ -912,37 +915,37 @@
       <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>40338</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>3.036744609778318E-2</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>4.2514424536896449</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>11.539629517157607</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>13.361676283024599</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>18.827816580625569</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>21.257212268448221</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <v>16.398420892802914</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>10.021257212268447</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <v>4.2514424536896449</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <v>6.073489219556636E-2</v>
       </c>
     </row>
@@ -968,37 +971,37 @@
       <c r="G8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>40703</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>7.9302141157811271E-2</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>9.516256938937353</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>13.481363996827914</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>15.860428231562254</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>18.239492466296593</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>19.825535289452816</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <v>11.102299762093578</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="2">
         <v>9.516256938937353</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>2.3790642347343383</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1024,37 +1027,37 @@
       <c r="G9" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>40703</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>0.20779220779220781</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>5.7142857142857144</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>18.181818181818183</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>19.220779220779221</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>17.662337662337663</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>18.181818181818183</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>14.545454545454545</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>5.1948051948051948</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>1.0389610389610389</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <v>5.1948051948051951E-2</v>
       </c>
     </row>
@@ -1080,37 +1083,37 @@
       <c r="G10" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>41069</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>8.404146045382388E-2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>12.139322065552339</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>15.874498085722289</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>23.344850126062187</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="2">
         <v>25.679335138668407</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="2">
         <v>14.006910075637313</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="2">
         <v>5.1358670277336813</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>2.3344850126062191</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="2">
         <v>1.4006910075637313</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1136,37 +1139,37 @@
       <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>41069</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>7.3264546065083341E-2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>12.699187984614447</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>12.821295561389585</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>13.431833445265278</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="2">
         <v>12.925087001648453</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>14.042371329140973</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="2">
         <v>15.263447096892364</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>12.02759631235118</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="2">
         <v>6.1053788387569456</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="2">
         <v>0.61053788387569452</v>
       </c>
     </row>
@@ -1192,37 +1195,37 @@
       <c r="G12" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>42235</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>0.13048817930610992</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>18.421860607921399</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>36.843721215842798</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>16.119128031931222</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="2">
         <v>11.513662879950875</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>8.4433527786306417</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="2">
         <v>5.1120663186981883</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>2.4101934295363834</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="2">
         <v>0.92109303039606993</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="2">
         <v>8.4433527786306417E-2</v>
       </c>
     </row>
@@ -1248,37 +1251,37 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <v>42235</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>0</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="2">
         <v>1.3066771200836274</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="2">
         <v>9.1467398405853917</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="2">
         <v>14.373448320919902</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="2">
         <v>19.600156801254411</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="2">
         <v>22.213511041421661</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="2">
         <v>18.594015418790015</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
         <v>12.805435776819548</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <v>1.9600156801254411</v>
       </c>
     </row>
@@ -1304,37 +1307,37 @@
       <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="3">
         <v>42235</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>0.10190563538163662</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>9.579129725873841</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>15.285845307245491</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>18.139203097931318</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="2">
         <v>18.34301436869459</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="2">
         <v>16.50871293182513</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="2">
         <v>11.209619891980028</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <v>7.4391113828594726</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="2">
         <v>3.2609803322123718</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="2">
         <v>0.1324773259961276</v>
       </c>
     </row>
@@ -1360,37 +1363,37 @@
       <c r="G15" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <v>42266</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>0.21299254526091588</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>10.649627263045794</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <v>12.779552715654955</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>15.974440894568692</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="2">
         <v>19.16932907348243</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="2">
         <v>16.293929712460066</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="2">
         <v>13.525026624068159</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="2">
         <v>10.756123535676251</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="2">
         <v>0.53248136315228967</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="2">
         <v>0.10649627263045794</v>
       </c>
     </row>
@@ -1416,37 +1419,37 @@
       <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>42296</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>0.11079104808331486</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>7.7553733658320398</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="2">
         <v>15.51074673166408</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <v>16.840239308663858</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="2">
         <v>11.189895856414802</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <v>13.073343673831154</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="2">
         <v>17.948149789497005</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="2">
         <v>11.85464214491469</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <v>5.5395524041657431</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="2">
         <v>0.17726567693330378</v>
       </c>
     </row>
@@ -1472,37 +1475,37 @@
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <v>42877</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>3.4799756401705184E-2</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>6.6699533103268278</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="2">
         <v>12.759910680625236</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="2">
         <v>16.239886320795755</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="2">
         <v>17.109880230838385</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="2">
         <v>14.789896470724706</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="2">
         <v>15.108894237740337</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="2">
         <v>12.237914334599658</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17" s="2">
         <v>4.9879650842444105</v>
       </c>
-      <c r="R17" s="3">
+      <c r="R17" s="2">
         <v>6.0899573702984079E-2</v>
       </c>
     </row>
@@ -1528,37 +1531,37 @@
       <c r="G18" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="3">
         <v>42877</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>3.5574528637495557E-2</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>6.0476698683742445</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="2">
         <v>11.383849163998578</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="2">
         <v>21.700462468872288</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18" s="2">
         <v>18.676627534685167</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="2">
         <v>16.293134115972965</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="2">
         <v>13.304873710423337</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2">
         <v>8.1821415866239775</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18" s="2">
         <v>4.2689434364994669</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <v>0.10672358591248667</v>
       </c>
     </row>
@@ -1584,37 +1587,37 @@
       <c r="G19" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="3">
         <v>42885</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>0</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>0</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="2">
         <v>0.15026296018031557</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="2">
         <v>0.75131480090157776</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="2">
         <v>6.8369646882043584</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="2">
         <v>18.03155522163787</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="2">
         <v>21.036814425244177</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2">
         <v>28.549962434259957</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19" s="2">
         <v>20.135236664162285</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <v>4.5078888054094675</v>
       </c>
     </row>
@@ -1640,37 +1643,37 @@
       <c r="G20" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <v>42898</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>6.1936259771497308</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>13.950691521346965</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="2">
         <v>19.663259170174388</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <v>19.843656043295251</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="2">
         <v>16.837041491280818</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="2">
         <v>15.033072760072161</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="2">
         <v>6.0132291040288637</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="2">
         <v>2.4052916416115453</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20" s="2">
         <v>6.0132291040288652E-2</v>
       </c>
-      <c r="R20" s="3">
+      <c r="R20" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1696,37 +1699,37 @@
       <c r="G21" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="3">
         <v>43705</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>0.10190563538163662</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>9.579129725873841</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="2">
         <v>15.285845307245491</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="2">
         <v>18.139203097931318</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="2">
         <v>18.34301436869459</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="2">
         <v>16.50871293182513</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="2">
         <v>11.209619891980028</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2">
         <v>7.4391113828594726</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="2">
         <v>3.2609803322123718</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21" s="2">
         <v>0.1324773259961276</v>
       </c>
     </row>

</xml_diff>